<commit_message>
Changed time period to only include 2019 data
</commit_message>
<xml_diff>
--- a/tri_data/table/tri_data_table.xlsx
+++ b/tri_data/table/tri_data_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tweiglein/Documents/Graduate School/Virginia Tech - Ph.D./IGC IGEP/RAAP/RAAP_transparency_project/tri_data/table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6DC78F-BEFC-3948-AAC0-ACE11CBCE118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA501103-6A9E-1445-80BA-32E36C269679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1520" windowWidth="27920" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>Chemical Name</t>
   </si>
@@ -28,67 +28,52 @@
     <t>Release Medium</t>
   </si>
   <si>
+    <t>Amount Released (lb)</t>
+  </si>
+  <si>
+    <t>Relative Contribution (%)</t>
+  </si>
+  <si>
     <t>Nitrate compounds</t>
   </si>
   <si>
     <t>Water</t>
   </si>
   <si>
-    <t>Hydrochloric acid</t>
+    <t>Nitroglycerin</t>
   </si>
   <si>
     <t>Air</t>
   </si>
   <si>
-    <t>Sulfuric acid</t>
-  </si>
-  <si>
-    <t>Nitroglycerin</t>
-  </si>
-  <si>
-    <t>Polycyclic aromatic compounds</t>
-  </si>
-  <si>
     <t>Ammonia</t>
   </si>
   <si>
+    <t>Nitric acid</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Copper compounds</t>
+  </si>
+  <si>
     <t>Lead compounds</t>
   </si>
   <si>
     <t>Off-site</t>
   </si>
   <si>
-    <t>Copper compounds</t>
-  </si>
-  <si>
-    <t>Nitric acid</t>
+    <t>Dibutyl phthalate</t>
+  </si>
+  <si>
+    <t>Mercury</t>
   </si>
   <si>
     <t>2 4-Dinitrotoluene</t>
   </si>
   <si>
-    <t>Land</t>
-  </si>
-  <si>
-    <t>Mercury</t>
-  </si>
-  <si>
-    <t>Dibutyl phthalate</t>
-  </si>
-  <si>
-    <t>Diphenylamine</t>
-  </si>
-  <si>
-    <t>Chlorine</t>
-  </si>
-  <si>
     <t>Dioxin and dioxin-like compounds</t>
-  </si>
-  <si>
-    <t>Total Releases [2010-2019] (lb)</t>
-  </si>
-  <si>
-    <t>Relative Contribution [2010-2019] (%)</t>
   </si>
 </sst>
 </file>
@@ -427,15 +412,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -445,137 +428,137 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>95497114</v>
+        <v>9119342</v>
       </c>
       <c r="D2" s="1">
-        <v>95.559862439167105</v>
+        <v>98.792184628475496</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>2459674</v>
+        <v>66543</v>
       </c>
       <c r="D3" s="1">
-        <v>2.46129018187079</v>
+        <v>0.72087748674549601</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2">
-        <v>514311.1</v>
+        <v>19294</v>
       </c>
       <c r="D4" s="1">
-        <v>0.51464903920485705</v>
+        <v>0.20901687975095201</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2">
-        <v>513944</v>
+        <v>9557</v>
       </c>
       <c r="D5" s="1">
-        <v>0.51428169799388201</v>
+        <v>0.10353344665594701</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
-        <v>361147.5</v>
+        <v>9275</v>
       </c>
       <c r="D6" s="1">
-        <v>0.36138479975687099</v>
+        <v>0.10047846790142401</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2">
-        <v>226341</v>
+        <v>2320</v>
       </c>
       <c r="D7" s="1">
-        <v>0.22648972223750699</v>
+        <v>2.5133158547849501E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
-        <v>139051.01</v>
+        <v>1461</v>
       </c>
       <c r="D8" s="1">
-        <v>0.139142376466238</v>
+        <v>1.5827389930348299E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2">
-        <v>90937.566739999995</v>
+        <v>1391.7</v>
       </c>
       <c r="D9" s="1">
-        <v>9.0997319230264703E-2</v>
+        <v>1.50766451513113E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2">
-        <v>30317</v>
+        <v>848.1</v>
       </c>
       <c r="D10" s="1">
-        <v>3.0336920438959299E-2</v>
+        <v>9.1876861053582694E-3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -583,41 +566,41 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2">
-        <v>18461.105</v>
+        <v>607.05999999999995</v>
       </c>
       <c r="D11" s="1">
-        <v>1.8473235267350799E-2</v>
+        <v>6.57643759830066E-3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
       <c r="C12" s="2">
-        <v>16022.2</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1">
-        <v>1.60327277321996E-2</v>
+        <v>6.7166199567528901E-4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2">
-        <v>15171.206</v>
+        <v>61.5</v>
       </c>
       <c r="D13" s="1">
-        <v>1.51811745682311E-2</v>
+        <v>6.6624536667790797E-4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -628,10 +611,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="2">
-        <v>14975.2</v>
+        <v>53.6</v>
       </c>
       <c r="D14" s="1">
-        <v>1.49850397782599E-2</v>
+        <v>5.8066262851928199E-4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -639,237 +622,69 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2">
-        <v>13129.9441491</v>
+        <v>9.5</v>
       </c>
       <c r="D15" s="1">
-        <v>1.31385714621904E-2</v>
+        <v>1.02915950950246E-4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
       <c r="C16" s="2">
-        <v>10957</v>
+        <v>7.92</v>
       </c>
       <c r="D16" s="1">
-        <v>1.09641995332545E-2</v>
+        <v>8.5799403318520803E-5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2">
-        <v>5467.6</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D17" s="1">
-        <v>5.4711926045470901E-3</v>
+        <v>2.7083144986906799E-7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2">
-        <v>4616.4650000000001</v>
+        <v>0.02</v>
       </c>
       <c r="D18" s="1">
-        <v>4.61949834793154E-3</v>
+        <v>2.1666515989525499E-7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C19" s="2">
-        <v>880.8</v>
+        <v>2.73E-5</v>
       </c>
       <c r="D19" s="1">
-        <v>8.8137874864384303E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="2">
-        <v>834.2</v>
-      </c>
-      <c r="D20" s="1">
-        <v>8.3474812910841695E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="2">
-        <v>370.66330219999998</v>
-      </c>
-      <c r="D21" s="1">
-        <v>3.70906854520016E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="2">
-        <v>311.60000000000002</v>
-      </c>
-      <c r="D22" s="1">
-        <v>3.1180474350297598E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2">
-        <v>99.9</v>
-      </c>
-      <c r="D23" s="1">
-        <v>9.99656414504086E-5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="2">
-        <v>89.8</v>
-      </c>
-      <c r="D24" s="1">
-        <v>8.9859005027494407E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2">
-        <v>75.905000000000001</v>
-      </c>
-      <c r="D25" s="1">
-        <v>7.5954875017950605E-5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="2">
-        <v>21.2</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2.1213929917404E-5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="2">
-        <v>9.6</v>
-      </c>
-      <c r="D27" s="1">
-        <v>9.6063078871263495E-6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D28" s="1">
-        <v>2.20144555746646E-6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2">
-        <v>2</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2.0013141431513199E-6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="D30" s="1">
-        <v>2.2014455574664601E-7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2">
-        <v>3.1981000000000002E-3</v>
-      </c>
-      <c r="D31" s="1">
-        <v>3.20020138060612E-9</v>
+        <v>2.9574794325702202E-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>